<commit_message>
make some notes, update endpoints
</commit_message>
<xml_diff>
--- a/4_standups/capstone_timeline.xlsx
+++ b/4_standups/capstone_timeline.xlsx
@@ -465,14 +465,14 @@
   <dimension ref="A4:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D5" sqref="C5:D5"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.6640625" style="4" customWidth="1"/>
     <col min="2" max="2" width="12.5" customWidth="1"/>
-    <col min="3" max="3" width="36.33203125" customWidth="1"/>
+    <col min="3" max="3" width="40.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="48.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="33.33203125" customWidth="1"/>
   </cols>
@@ -521,10 +521,10 @@
       <c r="B6" t="s">
         <v>1</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="5" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update toDos, buildapp, clean route_features.csv
</commit_message>
<xml_diff>
--- a/4_standups/capstone_timeline.xlsx
+++ b/4_standups/capstone_timeline.xlsx
@@ -465,7 +465,7 @@
   <dimension ref="A4:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -510,7 +510,7 @@
       <c r="D5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="5" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>